<commit_message>
raphie + justin instances in key
</commit_message>
<xml_diff>
--- a/InstanceKey.xlsx
+++ b/InstanceKey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="0" windowWidth="16160" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22840" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>ec2-54-183-246-23.us-west-1.compute.amazonaws.com</t>
   </si>
@@ -100,13 +100,64 @@
   </si>
   <si>
     <t>if stopped, -10, if crashed, -1, else linear(speed)</t>
+  </si>
+  <si>
+    <t>clipped loss, momentum = 0.95, "epsilon" = 0.01, clipped reward at 10</t>
+  </si>
+  <si>
+    <t>clipped loss, momentum = 0, clipped reward at 10</t>
+  </si>
+  <si>
+    <t>ec2-54-153-50-218.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t>Raphie</t>
+  </si>
+  <si>
+    <t>ec2-54-193-115-104.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ec2-54-193-76-3.us-west-1.compute.amazonaws.com </t>
+  </si>
+  <si>
+    <t>ec2-54-215-181-47.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t>ec2-54-193-93-156.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t>Adam + rishi reward function</t>
+  </si>
+  <si>
+    <t>no momentum + rishi reward function</t>
+  </si>
+  <si>
+    <t>momentum + rishi reward function</t>
+  </si>
+  <si>
+    <t>no momentum + raphie reward function</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>ec2-54-183-179-241.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t>ec2-54-193-26-113.us-west-1.compute.amazonaws.com</t>
+  </si>
+  <si>
+    <t>momentum + raphie reward</t>
+  </si>
+  <si>
+    <t>Adam + raphie reward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +193,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,8 +272,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,8 +315,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -251,6 +346,23 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -277,6 +389,23 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -636,82 +765,82 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>4</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -768,7 +897,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -780,15 +909,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="56" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -800,33 +929,135 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
+    <row r="37" spans="1:1">
+      <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>